<commit_message>
added few changes  3/09/2022
</commit_message>
<xml_diff>
--- a/SANTEGSMS/wwwroot/StudentBulkUpload (1).xlsx
+++ b/SANTEGSMS/wwwroot/StudentBulkUpload (1).xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P8623\Desktop\P8623\PP\SANTEGSMS\SANTEGSMS\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F686DF-FDAC-497C-A34D-415377AA0887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" xr2:uid="{64B60D9F-D0D0-467C-AFB6-863F031E958D}"/>
+    <workbookView xWindow="-120" yWindow="336" windowWidth="20736" windowHeight="11316"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
   <si>
     <t>Lastname</t>
   </si>
@@ -133,18 +132,9 @@
     <t>ABDULLAHI</t>
   </si>
   <si>
-    <t>AREMU</t>
-  </si>
-  <si>
-    <t>ABDULLAHIJOY021@yahoo.com</t>
-  </si>
-  <si>
     <t>Mr. ABDULLAHI</t>
   </si>
   <si>
-    <t>male</t>
-  </si>
-  <si>
     <t>lagos</t>
   </si>
   <si>
@@ -158,12 +148,54 @@
   </si>
   <si>
     <t>christian</t>
+  </si>
+  <si>
+    <t>Alade</t>
+  </si>
+  <si>
+    <t>Abiola</t>
+  </si>
+  <si>
+    <t>Olufunke</t>
+  </si>
+  <si>
+    <t>Akinkunmi</t>
+  </si>
+  <si>
+    <t>Olawale</t>
+  </si>
+  <si>
+    <t>Openiyi</t>
+  </si>
+  <si>
+    <t>Babatunde</t>
+  </si>
+  <si>
+    <t>Aremu</t>
+  </si>
+  <si>
+    <t>Asade</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>AremuAsade@yahoo.com</t>
+  </si>
+  <si>
+    <t>tundetunapa@@yahoo.com</t>
+  </si>
+  <si>
+    <t>Olawale099@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,41 +575,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD75D279-2F59-4335-9263-5B1ACA379D7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="6" max="6" width="33" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+    <col min="14" max="14" width="20.88671875" customWidth="1"/>
     <col min="15" max="16" width="23" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" customWidth="1"/>
     <col min="18" max="18" width="21" customWidth="1"/>
-    <col min="19" max="19" width="30.42578125" customWidth="1"/>
-    <col min="20" max="20" width="21.85546875" customWidth="1"/>
+    <col min="19" max="19" width="30.44140625" customWidth="1"/>
+    <col min="20" max="20" width="21.88671875" customWidth="1"/>
     <col min="21" max="21" width="19" customWidth="1"/>
-    <col min="22" max="22" width="21.5703125" customWidth="1"/>
+    <col min="22" max="22" width="21.5546875" customWidth="1"/>
     <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="19.5703125" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" customWidth="1"/>
-    <col min="26" max="26" width="18.42578125" customWidth="1"/>
+    <col min="24" max="24" width="19.5546875" customWidth="1"/>
+    <col min="25" max="25" width="18.5546875" customWidth="1"/>
+    <col min="26" max="26" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -657,18 +689,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>13</v>
@@ -680,10 +712,10 @@
         <v>2021</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>15</v>
@@ -698,16 +730,16 @@
         <v>14</v>
       </c>
       <c r="N2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
         <v>31</v>
       </c>
       <c r="P2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="R2">
         <v>9089897766</v>
@@ -725,61 +757,179 @@
         <v>16</v>
       </c>
       <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="X2" t="s">
+      <c r="C3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
+        <v>38691</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2021</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="7">
+        <v>9089897766</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="X3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" t="s">
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5">
+        <v>38691</v>
+      </c>
+      <c r="G4" s="7">
+        <v>2021</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R4" s="7">
+        <v>9089897766</v>
+      </c>
+      <c r="S4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z4" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
       <c r="H5" s="4"/>
@@ -800,7 +950,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
       <c r="H6" s="4"/>
@@ -821,7 +971,7 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
       <c r="H7" s="4"/>
@@ -842,7 +992,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="H8" s="4"/>
@@ -863,7 +1013,7 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="H9" s="4"/>
@@ -884,7 +1034,7 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="H10" s="4"/>
@@ -905,7 +1055,7 @@
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
       <c r="H11" s="4"/>
@@ -926,7 +1076,7 @@
       <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="H12" s="4"/>
@@ -947,7 +1097,7 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
       <c r="H13" s="4"/>
@@ -968,7 +1118,7 @@
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E14" s="4"/>
       <c r="F14" s="5"/>
       <c r="H14" s="4"/>
@@ -989,7 +1139,7 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E15" s="4"/>
       <c r="F15" s="5"/>
       <c r="H15" s="4"/>
@@ -1010,7 +1160,7 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
       <c r="H16" s="4"/>
@@ -1031,7 +1181,7 @@
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="H17" s="4"/>
@@ -1052,7 +1202,7 @@
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
     </row>
-    <row r="18" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E18" s="4"/>
       <c r="F18" s="5"/>
       <c r="H18" s="4"/>
@@ -1073,7 +1223,7 @@
       <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
     </row>
-    <row r="19" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="H19" s="4"/>
@@ -1094,7 +1244,7 @@
       <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
     </row>
-    <row r="20" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E20" s="4"/>
       <c r="F20" s="5"/>
       <c r="H20" s="4"/>
@@ -1115,7 +1265,7 @@
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E21" s="4"/>
       <c r="F21" s="5"/>
       <c r="H21" s="4"/>
@@ -1136,7 +1286,7 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
       <c r="H22" s="4"/>
@@ -1157,7 +1307,7 @@
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
     </row>
-    <row r="23" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E23" s="4"/>
       <c r="F23" s="5"/>
       <c r="H23" s="4"/>
@@ -1178,7 +1328,7 @@
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
     </row>
-    <row r="24" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
       <c r="H24" s="4"/>
@@ -1199,7 +1349,7 @@
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
     </row>
-    <row r="25" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
       <c r="H25" s="4"/>
@@ -1220,7 +1370,7 @@
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
     </row>
-    <row r="26" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E26" s="4"/>
       <c r="F26" s="5"/>
       <c r="H26" s="4"/>
@@ -1241,7 +1391,7 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
     </row>
-    <row r="27" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E27" s="4"/>
       <c r="F27" s="5"/>
       <c r="H27" s="4"/>
@@ -1262,7 +1412,7 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
     </row>
-    <row r="28" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E28" s="4"/>
       <c r="F28" s="5"/>
       <c r="H28" s="4"/>
@@ -1283,7 +1433,7 @@
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
     </row>
-    <row r="29" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E29" s="4"/>
       <c r="F29" s="5"/>
       <c r="H29" s="4"/>
@@ -1304,7 +1454,7 @@
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
     </row>
-    <row r="30" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E30" s="4"/>
       <c r="F30" s="5"/>
       <c r="H30" s="4"/>
@@ -1325,7 +1475,7 @@
       <c r="Y30" s="7"/>
       <c r="Z30" s="7"/>
     </row>
-    <row r="31" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
       <c r="H31" s="4"/>
@@ -1346,7 +1496,7 @@
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
     </row>
-    <row r="32" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
       <c r="H32" s="4"/>
@@ -1367,7 +1517,7 @@
       <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
     </row>
-    <row r="33" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
       <c r="H33" s="4"/>
@@ -1388,7 +1538,7 @@
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
     </row>
-    <row r="34" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E34" s="4"/>
       <c r="F34" s="5"/>
       <c r="H34" s="4"/>
@@ -1409,7 +1559,7 @@
       <c r="Y34" s="7"/>
       <c r="Z34" s="7"/>
     </row>
-    <row r="35" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E35" s="4"/>
       <c r="F35" s="5"/>
       <c r="H35" s="4"/>
@@ -1430,7 +1580,7 @@
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
     </row>
-    <row r="36" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E36" s="4"/>
       <c r="F36" s="5"/>
       <c r="H36" s="4"/>
@@ -1451,7 +1601,7 @@
       <c r="Y36" s="7"/>
       <c r="Z36" s="7"/>
     </row>
-    <row r="37" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E37" s="4"/>
       <c r="F37" s="5"/>
       <c r="H37" s="4"/>
@@ -1472,7 +1622,7 @@
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
     </row>
-    <row r="38" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E38" s="4"/>
       <c r="F38" s="5"/>
       <c r="H38" s="4"/>
@@ -1493,7 +1643,7 @@
       <c r="Y38" s="7"/>
       <c r="Z38" s="7"/>
     </row>
-    <row r="39" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
       <c r="H39" s="4"/>
@@ -1514,7 +1664,7 @@
       <c r="Y39" s="7"/>
       <c r="Z39" s="7"/>
     </row>
-    <row r="40" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E40" s="4"/>
       <c r="F40" s="5"/>
       <c r="H40" s="4"/>
@@ -1535,7 +1685,7 @@
       <c r="Y40" s="7"/>
       <c r="Z40" s="7"/>
     </row>
-    <row r="41" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E41" s="4"/>
       <c r="F41" s="5"/>
       <c r="H41" s="4"/>
@@ -1556,7 +1706,7 @@
       <c r="Y41" s="7"/>
       <c r="Z41" s="7"/>
     </row>
-    <row r="42" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="H42" s="4"/>
@@ -1577,7 +1727,7 @@
       <c r="Y42" s="7"/>
       <c r="Z42" s="7"/>
     </row>
-    <row r="43" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
       <c r="H43" s="4"/>
@@ -1598,7 +1748,7 @@
       <c r="Y43" s="7"/>
       <c r="Z43" s="7"/>
     </row>
-    <row r="44" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E44" s="4"/>
       <c r="F44" s="5"/>
       <c r="H44" s="4"/>
@@ -1619,7 +1769,7 @@
       <c r="Y44" s="7"/>
       <c r="Z44" s="7"/>
     </row>
-    <row r="45" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E45" s="4"/>
       <c r="F45" s="5"/>
       <c r="H45" s="4"/>
@@ -1640,7 +1790,7 @@
       <c r="Y45" s="7"/>
       <c r="Z45" s="7"/>
     </row>
-    <row r="46" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
       <c r="H46" s="4"/>
@@ -1661,7 +1811,7 @@
       <c r="Y46" s="7"/>
       <c r="Z46" s="7"/>
     </row>
-    <row r="47" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E47" s="4"/>
       <c r="F47" s="5"/>
       <c r="H47" s="4"/>
@@ -1682,7 +1832,7 @@
       <c r="Y47" s="7"/>
       <c r="Z47" s="7"/>
     </row>
-    <row r="48" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E48" s="4"/>
       <c r="F48" s="5"/>
       <c r="H48" s="4"/>
@@ -1703,7 +1853,7 @@
       <c r="Y48" s="7"/>
       <c r="Z48" s="7"/>
     </row>
-    <row r="49" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
       <c r="H49" s="4"/>
@@ -1724,7 +1874,7 @@
       <c r="Y49" s="7"/>
       <c r="Z49" s="7"/>
     </row>
-    <row r="50" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E50" s="4"/>
       <c r="F50" s="5"/>
       <c r="H50" s="4"/>
@@ -1745,7 +1895,7 @@
       <c r="Y50" s="7"/>
       <c r="Z50" s="7"/>
     </row>
-    <row r="51" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E51" s="4"/>
       <c r="F51" s="5"/>
       <c r="H51" s="4"/>
@@ -1766,7 +1916,7 @@
       <c r="Y51" s="7"/>
       <c r="Z51" s="7"/>
     </row>
-    <row r="52" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E52" s="4"/>
       <c r="F52" s="5"/>
       <c r="H52" s="4"/>
@@ -1787,7 +1937,7 @@
       <c r="Y52" s="7"/>
       <c r="Z52" s="7"/>
     </row>
-    <row r="53" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E53" s="4"/>
       <c r="F53" s="5"/>
       <c r="H53" s="4"/>
@@ -1808,7 +1958,7 @@
       <c r="Y53" s="7"/>
       <c r="Z53" s="7"/>
     </row>
-    <row r="54" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E54" s="4"/>
       <c r="F54" s="5"/>
       <c r="H54" s="4"/>
@@ -1829,7 +1979,7 @@
       <c r="Y54" s="7"/>
       <c r="Z54" s="7"/>
     </row>
-    <row r="55" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E55" s="4"/>
       <c r="F55" s="5"/>
       <c r="H55" s="4"/>
@@ -1850,7 +2000,7 @@
       <c r="Y55" s="7"/>
       <c r="Z55" s="7"/>
     </row>
-    <row r="56" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E56" s="4"/>
       <c r="F56" s="5"/>
       <c r="H56" s="4"/>
@@ -1871,7 +2021,7 @@
       <c r="Y56" s="7"/>
       <c r="Z56" s="7"/>
     </row>
-    <row r="57" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="H57" s="4"/>
@@ -1892,7 +2042,7 @@
       <c r="Y57" s="7"/>
       <c r="Z57" s="7"/>
     </row>
-    <row r="58" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E58" s="4"/>
       <c r="F58" s="5"/>
       <c r="H58" s="4"/>
@@ -1913,7 +2063,7 @@
       <c r="Y58" s="7"/>
       <c r="Z58" s="7"/>
     </row>
-    <row r="59" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E59" s="4"/>
       <c r="F59" s="5"/>
       <c r="H59" s="4"/>
@@ -1934,7 +2084,7 @@
       <c r="Y59" s="7"/>
       <c r="Z59" s="7"/>
     </row>
-    <row r="60" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E60" s="4"/>
       <c r="F60" s="5"/>
       <c r="H60" s="4"/>
@@ -1955,7 +2105,7 @@
       <c r="Y60" s="7"/>
       <c r="Z60" s="7"/>
     </row>
-    <row r="61" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E61" s="4"/>
       <c r="F61" s="5"/>
       <c r="H61" s="4"/>
@@ -1976,7 +2126,7 @@
       <c r="Y61" s="7"/>
       <c r="Z61" s="7"/>
     </row>
-    <row r="62" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E62" s="4"/>
       <c r="F62" s="5"/>
       <c r="H62" s="4"/>
@@ -1997,7 +2147,7 @@
       <c r="Y62" s="7"/>
       <c r="Z62" s="7"/>
     </row>
-    <row r="63" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
       <c r="H63" s="4"/>
@@ -2018,7 +2168,7 @@
       <c r="Y63" s="7"/>
       <c r="Z63" s="7"/>
     </row>
-    <row r="64" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E64" s="4"/>
       <c r="F64" s="5"/>
       <c r="H64" s="4"/>
@@ -2039,7 +2189,7 @@
       <c r="Y64" s="7"/>
       <c r="Z64" s="7"/>
     </row>
-    <row r="65" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E65" s="4"/>
       <c r="F65" s="5"/>
       <c r="H65" s="4"/>
@@ -2060,7 +2210,7 @@
       <c r="Y65" s="7"/>
       <c r="Z65" s="7"/>
     </row>
-    <row r="66" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E66" s="4"/>
       <c r="F66" s="5"/>
       <c r="H66" s="4"/>
@@ -2081,7 +2231,7 @@
       <c r="Y66" s="7"/>
       <c r="Z66" s="7"/>
     </row>
-    <row r="67" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E67" s="4"/>
       <c r="F67" s="5"/>
       <c r="H67" s="4"/>
@@ -2102,7 +2252,7 @@
       <c r="Y67" s="7"/>
       <c r="Z67" s="7"/>
     </row>
-    <row r="68" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E68" s="4"/>
       <c r="F68" s="5"/>
       <c r="H68" s="4"/>
@@ -2123,7 +2273,7 @@
       <c r="Y68" s="7"/>
       <c r="Z68" s="7"/>
     </row>
-    <row r="69" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E69" s="4"/>
       <c r="F69" s="5"/>
       <c r="H69" s="4"/>
@@ -2144,7 +2294,7 @@
       <c r="Y69" s="7"/>
       <c r="Z69" s="7"/>
     </row>
-    <row r="70" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E70" s="4"/>
       <c r="F70" s="5"/>
       <c r="H70" s="4"/>
@@ -2165,7 +2315,7 @@
       <c r="Y70" s="7"/>
       <c r="Z70" s="7"/>
     </row>
-    <row r="71" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E71" s="4"/>
       <c r="F71" s="5"/>
       <c r="H71" s="4"/>
@@ -2186,7 +2336,7 @@
       <c r="Y71" s="7"/>
       <c r="Z71" s="7"/>
     </row>
-    <row r="72" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E72" s="4"/>
       <c r="F72" s="5"/>
       <c r="H72" s="4"/>
@@ -2207,7 +2357,7 @@
       <c r="Y72" s="7"/>
       <c r="Z72" s="7"/>
     </row>
-    <row r="73" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E73" s="4"/>
       <c r="F73" s="5"/>
       <c r="H73" s="4"/>
@@ -2228,7 +2378,7 @@
       <c r="Y73" s="7"/>
       <c r="Z73" s="7"/>
     </row>
-    <row r="74" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E74" s="4"/>
       <c r="F74" s="5"/>
       <c r="H74" s="4"/>
@@ -2249,7 +2399,7 @@
       <c r="Y74" s="7"/>
       <c r="Z74" s="7"/>
     </row>
-    <row r="75" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E75" s="4"/>
       <c r="F75" s="5"/>
       <c r="H75" s="4"/>
@@ -2270,7 +2420,7 @@
       <c r="Y75" s="7"/>
       <c r="Z75" s="7"/>
     </row>
-    <row r="76" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E76" s="4"/>
       <c r="F76" s="5"/>
       <c r="H76" s="4"/>
@@ -2291,7 +2441,7 @@
       <c r="Y76" s="7"/>
       <c r="Z76" s="7"/>
     </row>
-    <row r="77" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E77" s="4"/>
       <c r="F77" s="5"/>
       <c r="H77" s="4"/>
@@ -2312,7 +2462,7 @@
       <c r="Y77" s="7"/>
       <c r="Z77" s="7"/>
     </row>
-    <row r="78" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E78" s="4"/>
       <c r="F78" s="5"/>
       <c r="H78" s="4"/>
@@ -2333,7 +2483,7 @@
       <c r="Y78" s="7"/>
       <c r="Z78" s="7"/>
     </row>
-    <row r="79" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E79" s="4"/>
       <c r="F79" s="5"/>
       <c r="H79" s="4"/>
@@ -2354,7 +2504,7 @@
       <c r="Y79" s="7"/>
       <c r="Z79" s="7"/>
     </row>
-    <row r="80" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E80" s="4"/>
       <c r="F80" s="5"/>
       <c r="H80" s="4"/>
@@ -2375,7 +2525,7 @@
       <c r="Y80" s="7"/>
       <c r="Z80" s="7"/>
     </row>
-    <row r="81" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E81" s="4"/>
       <c r="F81" s="5"/>
       <c r="H81" s="4"/>
@@ -2396,7 +2546,7 @@
       <c r="Y81" s="7"/>
       <c r="Z81" s="7"/>
     </row>
-    <row r="82" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E82" s="4"/>
       <c r="F82" s="5"/>
       <c r="H82" s="4"/>
@@ -2417,7 +2567,7 @@
       <c r="Y82" s="7"/>
       <c r="Z82" s="7"/>
     </row>
-    <row r="83" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E83" s="4"/>
       <c r="F83" s="5"/>
       <c r="H83" s="4"/>
@@ -2438,7 +2588,7 @@
       <c r="Y83" s="7"/>
       <c r="Z83" s="7"/>
     </row>
-    <row r="84" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E84" s="4"/>
       <c r="F84" s="5"/>
       <c r="H84" s="4"/>
@@ -2459,7 +2609,7 @@
       <c r="Y84" s="7"/>
       <c r="Z84" s="7"/>
     </row>
-    <row r="85" spans="5:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:26" x14ac:dyDescent="0.3">
       <c r="E85" s="4"/>
       <c r="F85" s="5"/>
       <c r="H85" s="4"/>
@@ -2482,7 +2632,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1"/>
+    <hyperlink ref="Q3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>